<commit_message>
Fixed dates in ccw_lookup column
</commit_message>
<xml_diff>
--- a/claims_data/ccw_lookup.xlsx
+++ b/claims_data/ccw_lookup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kc1-my.sharepoint.com/personal/alastair_matheson_kingcounty_gov/Documents/github/reference-data/claims_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="406" documentId="11_9A33B9A22B7DCD35061FD0B4DF8B81B7DEB0F1C7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A93151B-F564-44ED-9111-920376BFC235}"/>
+  <xr:revisionPtr revIDLastSave="408" documentId="11_9A33B9A22B7DCD35061FD0B4DF8B81B7DEB0F1C7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75CA8450-0D95-4117-9CCD-4BDA3B446AD1}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="label" sheetId="4" state="hidden" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9099" uniqueCount="4316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9129" uniqueCount="4316">
   <si>
     <t>Acquired Hypothyrodism</t>
   </si>
@@ -73076,7 +73076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D624538-775A-4896-8368-5AB97255472E}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -74277,8 +74277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -74344,8 +74344,8 @@
       <c r="D2" s="3" t="s">
         <v>1197</v>
       </c>
-      <c r="E2" s="11">
-        <v>43497</v>
+      <c r="E2" s="11" t="s">
+        <v>4307</v>
       </c>
       <c r="F2" s="3">
         <v>1</v>
@@ -74379,8 +74379,8 @@
       <c r="D3" s="3" t="s">
         <v>1198</v>
       </c>
-      <c r="E3" s="11">
-        <v>43497</v>
+      <c r="E3" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F3" s="3">
         <v>1</v>
@@ -74411,8 +74411,8 @@
       <c r="D4" s="12" t="s">
         <v>1199</v>
       </c>
-      <c r="E4" s="11">
-        <v>43497</v>
+      <c r="E4" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F4" s="12">
         <v>3</v>
@@ -74443,8 +74443,8 @@
       <c r="D5" s="3" t="s">
         <v>1200</v>
       </c>
-      <c r="E5" s="11">
-        <v>43497</v>
+      <c r="E5" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F5" s="3">
         <v>3</v>
@@ -74475,8 +74475,8 @@
       <c r="D6" s="3" t="s">
         <v>1201</v>
       </c>
-      <c r="E6" s="11">
-        <v>43497</v>
+      <c r="E6" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F6" s="3">
         <v>1</v>
@@ -74507,8 +74507,8 @@
       <c r="D7" s="3" t="s">
         <v>1156</v>
       </c>
-      <c r="E7" s="11">
-        <v>43497</v>
+      <c r="E7" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F7" s="3">
         <v>1</v>
@@ -74542,8 +74542,8 @@
       <c r="D8" s="3" t="s">
         <v>1202</v>
       </c>
-      <c r="E8" s="11">
-        <v>43497</v>
+      <c r="E8" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F8" s="3">
         <v>1</v>
@@ -74577,8 +74577,8 @@
       <c r="D9" s="3" t="s">
         <v>1203</v>
       </c>
-      <c r="E9" s="11">
-        <v>43497</v>
+      <c r="E9" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F9" s="10">
         <v>1</v>
@@ -74612,8 +74612,8 @@
       <c r="D10" s="3" t="s">
         <v>1437</v>
       </c>
-      <c r="E10" s="11">
-        <v>43497</v>
+      <c r="E10" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
@@ -74647,8 +74647,8 @@
       <c r="D11" s="3" t="s">
         <v>1193</v>
       </c>
-      <c r="E11" s="11">
-        <v>43497</v>
+      <c r="E11" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F11" s="10">
         <v>1</v>
@@ -74679,8 +74679,8 @@
       <c r="D12" s="3" t="s">
         <v>1160</v>
       </c>
-      <c r="E12" s="11">
-        <v>43497</v>
+      <c r="E12" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F12" s="3">
         <v>2</v>
@@ -74714,8 +74714,8 @@
       <c r="D13" s="3" t="s">
         <v>1204</v>
       </c>
-      <c r="E13" s="11">
-        <v>43497</v>
+      <c r="E13" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F13" s="3">
         <v>1</v>
@@ -74749,8 +74749,8 @@
       <c r="D14" s="3" t="s">
         <v>1157</v>
       </c>
-      <c r="E14" s="11">
-        <v>43497</v>
+      <c r="E14" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F14" s="3">
         <v>1</v>
@@ -74784,8 +74784,8 @@
       <c r="D15" s="3" t="s">
         <v>1155</v>
       </c>
-      <c r="E15" s="11">
-        <v>43497</v>
+      <c r="E15" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F15" s="3">
         <v>1</v>
@@ -74816,8 +74816,8 @@
       <c r="D16" s="3" t="s">
         <v>1158</v>
       </c>
-      <c r="E16" s="11">
-        <v>43497</v>
+      <c r="E16" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F16" s="3">
         <v>2</v>
@@ -74851,8 +74851,8 @@
       <c r="D17" s="3" t="s">
         <v>1205</v>
       </c>
-      <c r="E17" s="11">
-        <v>43497</v>
+      <c r="E17" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F17" s="3">
         <v>1</v>
@@ -74886,8 +74886,8 @@
       <c r="D18" s="3" t="s">
         <v>1208</v>
       </c>
-      <c r="E18" s="11">
-        <v>43497</v>
+      <c r="E18" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F18" s="3">
         <v>1</v>
@@ -74921,8 +74921,8 @@
       <c r="D19" s="3" t="s">
         <v>1194</v>
       </c>
-      <c r="E19" s="11">
-        <v>43497</v>
+      <c r="E19" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F19" s="10">
         <v>1</v>
@@ -74953,8 +74953,8 @@
       <c r="D20" s="3" t="s">
         <v>1154</v>
       </c>
-      <c r="E20" s="11">
-        <v>43497</v>
+      <c r="E20" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F20" s="3">
         <v>2</v>
@@ -74985,8 +74985,8 @@
       <c r="D21" s="3" t="s">
         <v>1196</v>
       </c>
-      <c r="E21" s="11">
-        <v>43497</v>
+      <c r="E21" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F21" s="10">
         <v>1</v>
@@ -75017,8 +75017,8 @@
       <c r="D22" s="3" t="s">
         <v>1209</v>
       </c>
-      <c r="E22" s="11">
-        <v>43497</v>
+      <c r="E22" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F22" s="10">
         <v>1</v>
@@ -75052,8 +75052,8 @@
       <c r="D23" s="3" t="s">
         <v>1159</v>
       </c>
-      <c r="E23" s="11">
-        <v>43497</v>
+      <c r="E23" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F23" s="3">
         <v>1</v>
@@ -75087,8 +75087,8 @@
       <c r="D24" s="3" t="s">
         <v>1153</v>
       </c>
-      <c r="E24" s="11">
-        <v>43497</v>
+      <c r="E24" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F24" s="3">
         <v>2</v>
@@ -75119,8 +75119,8 @@
       <c r="D25" s="3" t="s">
         <v>1206</v>
       </c>
-      <c r="E25" s="11">
-        <v>43497</v>
+      <c r="E25" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F25" s="3">
         <v>1</v>
@@ -75154,8 +75154,8 @@
       <c r="D26" s="3" t="s">
         <v>1195</v>
       </c>
-      <c r="E26" s="11">
-        <v>43497</v>
+      <c r="E26" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F26" s="10">
         <v>1</v>
@@ -75189,8 +75189,8 @@
       <c r="D27" s="3" t="s">
         <v>1207</v>
       </c>
-      <c r="E27" s="11">
-        <v>43497</v>
+      <c r="E27" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F27" s="3">
         <v>1</v>
@@ -75224,8 +75224,8 @@
       <c r="D28" s="3" t="s">
         <v>1210</v>
       </c>
-      <c r="E28" s="11">
-        <v>43497</v>
+      <c r="E28" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F28" s="10">
         <v>2</v>
@@ -75256,8 +75256,8 @@
       <c r="D29" s="3" t="s">
         <v>1211</v>
       </c>
-      <c r="E29" s="11">
-        <v>43497</v>
+      <c r="E29" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F29" s="10">
         <v>1</v>
@@ -75291,8 +75291,8 @@
       <c r="D30" s="3" t="s">
         <v>3110</v>
       </c>
-      <c r="E30" s="11">
-        <v>43497</v>
+      <c r="E30" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F30" s="3">
         <v>1</v>
@@ -75326,8 +75326,8 @@
       <c r="D31" s="3" t="s">
         <v>3112</v>
       </c>
-      <c r="E31" s="11">
-        <v>43497</v>
+      <c r="E31" s="26" t="s">
+        <v>4307</v>
       </c>
       <c r="F31" s="3">
         <v>1</v>
@@ -76417,12 +76417,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010098C197DC67C0514EB308983AEF32E983" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a506a90b446ec8f6ca9341c1992a61de">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d55fa3f-3c18-425b-9faa-377f011f8097" xmlns:ns3="39d3cee1-f650-41e8-9a2f-4357c6682977" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="68eb73591874d7b6cee55945c0a8d5bf" ns2:_="" ns3:_="">
     <xsd:import namespace="3d55fa3f-3c18-425b-9faa-377f011f8097"/>
@@ -76599,6 +76593,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76AD4B54-6DC2-4D8C-86CA-5908AE6EF015}">
   <ds:schemaRefs>
@@ -76608,23 +76608,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC2EEFE0-2F39-4B6B-9A9A-7092F0DE0B00}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="3d55fa3f-3c18-425b-9faa-377f011f8097"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="39d3cee1-f650-41e8-9a2f-4357c6682977"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A61351A-2F7F-48FB-A782-AE9A92A10B40}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -76641,4 +76624,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC2EEFE0-2F39-4B6B-9A9A-7092F0DE0B00}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="3d55fa3f-3c18-425b-9faa-377f011f8097"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="39d3cee1-f650-41e8-9a2f-4357c6682977"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Standardized ccw_lookup column names to match SQL table
</commit_message>
<xml_diff>
--- a/claims_data/ccw_lookup.xlsx
+++ b/claims_data/ccw_lookup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kc1-my.sharepoint.com/personal/alastair_matheson_kingcounty_gov/Documents/github/reference-data/claims_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="408" documentId="11_9A33B9A22B7DCD35061FD0B4DF8B81B7DEB0F1C7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75CA8450-0D95-4117-9CCD-4BDA3B446AD1}"/>
+  <xr:revisionPtr revIDLastSave="422" documentId="11_9A33B9A22B7DCD35061FD0B4DF8B81B7DEB0F1C7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4232A6AB-71BE-46C1-82B5-A6AC244D755F}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9129" uniqueCount="4316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9129" uniqueCount="4321">
   <si>
     <t>Acquired Hypothyrodism</t>
   </si>
@@ -12907,15 +12907,6 @@
   </si>
   <si>
     <t>ccw qualification types</t>
-  </si>
-  <si>
-    <t>claim_type1 = types of claim that need 1 visit in the lookback period</t>
-  </si>
-  <si>
-    <t>claim_type2 = types of claim that need 2 visits in the lookback period</t>
-  </si>
-  <si>
-    <t>condition type = if all claims type only need 1 visit (=1) or some claim types need 2 visits (=2) in lookback period. Used to set up SQL code in claim_ccw function (https://github.com/PHSKC-APDE/claims_data/blob/main/claims_db/db_loader/scripts_general/claim_ccw.R).</t>
   </si>
   <si>
     <t>ccw_definitions_p1</t>
@@ -13020,6 +13011,30 @@
   </si>
   <si>
     <t>ccw_icd_version</t>
+  </si>
+  <si>
+    <t>ccw_version</t>
+  </si>
+  <si>
+    <t>dx_fields</t>
+  </si>
+  <si>
+    <t>condition_type</t>
+  </si>
+  <si>
+    <t>claim_type_1</t>
+  </si>
+  <si>
+    <t>claim_type_2</t>
+  </si>
+  <si>
+    <t>claim_type_1 = types of claim that need 1 visit in the lookback period</t>
+  </si>
+  <si>
+    <t>claim_type_2 = types of claim that need 2 visits in the lookback period</t>
+  </si>
+  <si>
+    <t>condition_type = if all claims type only need 1 visit (=1) or some claim types need 2 visits (=2) in lookback period. Used to set up SQL code in claim_ccw function (https://github.com/PHSKC-APDE/claims_data/blob/main/claims_db/db_loader/scripts_general/claim_ccw.R).</t>
   </si>
 </sst>
 </file>
@@ -13119,7 +13134,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -13185,9 +13200,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -73077,7 +73089,7 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -73086,7 +73098,7 @@
     <col min="2" max="2" width="13.3984375" style="3" customWidth="1"/>
     <col min="3" max="3" width="49.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" style="3" customWidth="1"/>
-    <col min="5" max="5" width="15.265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="15.265625" style="26" customWidth="1"/>
     <col min="6" max="6" width="11.1328125" style="3" customWidth="1"/>
     <col min="7" max="7" width="13.86328125" style="14" customWidth="1"/>
     <col min="8" max="8" width="70.265625" style="4" customWidth="1"/>
@@ -73097,37 +73109,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="18" t="s">
+        <v>4312</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>1191</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>4313</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>4314</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>4316</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>4317</v>
+      </c>
+      <c r="K1" s="24" t="s">
         <v>4315</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>1191</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>1192</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>1145</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>1146</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>1151</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
@@ -73143,7 +73155,7 @@
       <c r="D2" s="3" t="s">
         <v>1197</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F2" s="3">
@@ -73156,10 +73168,10 @@
         <v>44</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>4298</v>
+        <v>4295</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K2" s="3">
         <v>2</v>
@@ -73178,7 +73190,7 @@
       <c r="D3" s="3" t="s">
         <v>1198</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F3" s="3">
@@ -73210,7 +73222,7 @@
       <c r="D4" s="12" t="s">
         <v>1199</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F4" s="12">
@@ -73223,10 +73235,10 @@
         <v>44</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>4298</v>
+        <v>4295</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K4" s="3">
         <v>2</v>
@@ -73245,8 +73257,8 @@
       <c r="D5" s="3" t="s">
         <v>1200</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>4307</v>
+      <c r="E5" s="26" t="s">
+        <v>4304</v>
       </c>
       <c r="F5" s="3">
         <v>3</v>
@@ -73258,7 +73270,7 @@
         <v>46</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>4300</v>
+        <v>4297</v>
       </c>
       <c r="K5" s="3">
         <v>1</v>
@@ -73277,7 +73289,7 @@
       <c r="D6" s="3" t="s">
         <v>1201</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F6" s="3">
@@ -73290,10 +73302,10 @@
         <v>44</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>4298</v>
+        <v>4295</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K6" s="3">
         <v>2</v>
@@ -73312,7 +73324,7 @@
       <c r="D7" s="3" t="s">
         <v>1156</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F7" s="3">
@@ -73325,10 +73337,10 @@
         <v>44</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>4298</v>
+        <v>4295</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K7" s="9">
         <v>2</v>
@@ -73347,7 +73359,7 @@
       <c r="D8" s="3" t="s">
         <v>1202</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F8" s="3">
@@ -73360,10 +73372,10 @@
         <v>44</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>4298</v>
+        <v>4295</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K8" s="9">
         <v>2</v>
@@ -73382,7 +73394,7 @@
       <c r="D9" s="3" t="s">
         <v>1203</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F9" s="10">
@@ -73395,10 +73407,10 @@
         <v>44</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>4298</v>
+        <v>4295</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K9" s="9">
         <v>2</v>
@@ -73417,7 +73429,7 @@
       <c r="D10" s="3" t="s">
         <v>1437</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F10" s="10">
@@ -73430,10 +73442,10 @@
         <v>44</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>4298</v>
+        <v>4295</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K10" s="9">
         <v>2</v>
@@ -73452,7 +73464,7 @@
       <c r="D11" s="3" t="s">
         <v>1193</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F11" s="10">
@@ -73465,7 +73477,7 @@
         <v>3914</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K11" s="3">
         <v>1</v>
@@ -73484,7 +73496,7 @@
       <c r="D12" s="3" t="s">
         <v>1160</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F12" s="3">
@@ -73497,10 +73509,10 @@
         <v>44</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>4298</v>
+        <v>4295</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K12" s="9">
         <v>2</v>
@@ -73519,7 +73531,7 @@
       <c r="D13" s="3" t="s">
         <v>1204</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F13" s="3">
@@ -73532,10 +73544,10 @@
         <v>3915</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>4302</v>
+        <v>4299</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K13" s="3">
         <v>2</v>
@@ -73554,7 +73566,7 @@
       <c r="D14" s="3" t="s">
         <v>1157</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F14" s="3">
@@ -73567,10 +73579,10 @@
         <v>44</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>4298</v>
+        <v>4295</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K14" s="9">
         <v>2</v>
@@ -73589,7 +73601,7 @@
       <c r="D15" s="3" t="s">
         <v>1155</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F15" s="3">
@@ -73602,10 +73614,10 @@
         <v>44</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>4298</v>
+        <v>4295</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K15" s="9">
         <v>2</v>
@@ -73624,7 +73636,7 @@
       <c r="D16" s="3" t="s">
         <v>1158</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F16" s="3">
@@ -73637,10 +73649,10 @@
         <v>44</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>4298</v>
+        <v>4295</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K16" s="9">
         <v>2</v>
@@ -73659,7 +73671,7 @@
       <c r="D17" s="3" t="s">
         <v>1205</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F17" s="3">
@@ -73672,10 +73684,10 @@
         <v>3915</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>4302</v>
+        <v>4299</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K17" s="3">
         <v>2</v>
@@ -73694,7 +73706,7 @@
       <c r="D18" s="3" t="s">
         <v>1208</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F18" s="3">
@@ -73707,10 +73719,10 @@
         <v>3915</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>4302</v>
+        <v>4299</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K18" s="3">
         <v>2</v>
@@ -73729,7 +73741,7 @@
       <c r="D19" s="3" t="s">
         <v>1194</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F19" s="10">
@@ -73742,7 +73754,7 @@
         <v>3914</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K19" s="3">
         <v>1</v>
@@ -73761,7 +73773,7 @@
       <c r="D20" s="3" t="s">
         <v>1154</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F20" s="3">
@@ -73774,10 +73786,10 @@
         <v>44</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>4298</v>
+        <v>4295</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K20" s="9">
         <v>2</v>
@@ -73796,7 +73808,7 @@
       <c r="D21" s="3" t="s">
         <v>1196</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F21" s="10">
@@ -73806,10 +73818,10 @@
         <v>38</v>
       </c>
       <c r="H21" s="21" t="s">
-        <v>4297</v>
+        <v>4294</v>
       </c>
       <c r="I21" s="25" t="s">
-        <v>4303</v>
+        <v>4300</v>
       </c>
       <c r="J21" s="20"/>
       <c r="K21" s="20">
@@ -73829,7 +73841,7 @@
       <c r="D22" s="3" t="s">
         <v>1209</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F22" s="10">
@@ -73842,10 +73854,10 @@
         <v>44</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>4298</v>
+        <v>4295</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K22" s="3">
         <v>2</v>
@@ -73864,7 +73876,7 @@
       <c r="D23" s="3" t="s">
         <v>1159</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F23" s="3">
@@ -73877,10 +73889,10 @@
         <v>44</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>4298</v>
+        <v>4295</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K23" s="9">
         <v>2</v>
@@ -73899,7 +73911,7 @@
       <c r="D24" s="3" t="s">
         <v>1153</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F24" s="3">
@@ -73912,10 +73924,10 @@
         <v>44</v>
       </c>
       <c r="I24" s="20" t="s">
-        <v>4298</v>
+        <v>4295</v>
       </c>
       <c r="J24" s="20" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K24" s="25">
         <v>2</v>
@@ -73934,7 +73946,7 @@
       <c r="D25" s="3" t="s">
         <v>1206</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F25" s="3">
@@ -73947,10 +73959,10 @@
         <v>3915</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>4302</v>
+        <v>4299</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K25" s="3">
         <v>2</v>
@@ -73964,12 +73976,12 @@
         <v>24</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>4305</v>
+        <v>4302</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>1195</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F26" s="10">
@@ -73982,10 +73994,10 @@
         <v>44</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>4298</v>
+        <v>4295</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K26" s="3">
         <v>2</v>
@@ -74004,7 +74016,7 @@
       <c r="D27" s="3" t="s">
         <v>1207</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F27" s="3">
@@ -74017,10 +74029,10 @@
         <v>3915</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>4302</v>
+        <v>4299</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K27" s="3">
         <v>2</v>
@@ -74039,7 +74051,7 @@
       <c r="D28" s="3" t="s">
         <v>1210</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F28" s="10">
@@ -74052,10 +74064,10 @@
         <v>44</v>
       </c>
       <c r="I28" s="20" t="s">
-        <v>4298</v>
+        <v>4295</v>
       </c>
       <c r="J28" s="20" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K28" s="20">
         <v>2</v>
@@ -74074,7 +74086,7 @@
       <c r="D29" s="3" t="s">
         <v>1211</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F29" s="10">
@@ -74107,7 +74119,7 @@
       <c r="D30" s="3" t="s">
         <v>3110</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F30" s="3">
@@ -74140,7 +74152,7 @@
       <c r="D31" s="3" t="s">
         <v>3980</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F31" s="3">
@@ -74153,10 +74165,10 @@
         <v>3915</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>4302</v>
+        <v>4299</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K31" s="3">
         <v>2</v>
@@ -74170,28 +74182,28 @@
         <v>29</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>4304</v>
+        <v>4301</v>
       </c>
       <c r="D32" s="20" t="s">
         <v>4046</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F32" s="3">
         <v>2</v>
       </c>
-      <c r="G32" s="27" t="s">
+      <c r="G32" s="26" t="s">
         <v>38</v>
       </c>
       <c r="H32" s="21" t="s">
         <v>44</v>
       </c>
       <c r="I32" s="20" t="s">
-        <v>4298</v>
+        <v>4295</v>
       </c>
       <c r="J32" s="20" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K32" s="20">
         <v>2</v>
@@ -74205,28 +74217,28 @@
         <v>30</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>4306</v>
+        <v>4303</v>
       </c>
       <c r="D33" s="20" t="s">
         <v>4089</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="26" t="s">
         <v>4270</v>
       </c>
       <c r="F33" s="3">
         <v>2</v>
       </c>
-      <c r="G33" s="27" t="s">
+      <c r="G33" s="26" t="s">
         <v>38</v>
       </c>
       <c r="H33" s="21" t="s">
         <v>44</v>
       </c>
       <c r="I33" s="20" t="s">
-        <v>4298</v>
+        <v>4295</v>
       </c>
       <c r="J33" s="20" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K33" s="20">
         <v>2</v>
@@ -74240,7 +74252,7 @@
         <v>31</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>4308</v>
+        <v>4305</v>
       </c>
       <c r="D34" s="20" t="s">
         <v>4188</v>
@@ -74251,17 +74263,17 @@
       <c r="F34" s="3">
         <v>1</v>
       </c>
-      <c r="G34" s="27" t="s">
+      <c r="G34" s="26" t="s">
         <v>38</v>
       </c>
       <c r="H34" s="21" t="s">
         <v>44</v>
       </c>
       <c r="I34" s="20" t="s">
-        <v>4298</v>
+        <v>4295</v>
       </c>
       <c r="J34" s="20" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="K34" s="20">
         <v>2</v>
@@ -74275,10 +74287,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E31"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -74287,7 +74299,7 @@
     <col min="2" max="2" width="13.3984375" style="3" customWidth="1"/>
     <col min="3" max="3" width="49.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" style="3" customWidth="1"/>
-    <col min="5" max="5" width="15.265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="15.265625" style="26" customWidth="1"/>
     <col min="6" max="6" width="11.1328125" style="3" customWidth="1"/>
     <col min="7" max="7" width="13.86328125" style="14" customWidth="1"/>
     <col min="8" max="8" width="70.265625" style="4" customWidth="1"/>
@@ -74298,7 +74310,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="18" t="s">
-        <v>4315</v>
+        <v>4312</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>71</v>
@@ -74309,26 +74321,26 @@
       <c r="D1" s="6" t="s">
         <v>1192</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>76</v>
+      <c r="E1" s="15" t="s">
+        <v>4313</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>37</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>77</v>
+        <v>4314</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>78</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>1145</v>
+        <v>4316</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>1146</v>
+        <v>4317</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>1151</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
@@ -74344,8 +74356,8 @@
       <c r="D2" s="3" t="s">
         <v>1197</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>4307</v>
+      <c r="E2" s="26" t="s">
+        <v>4304</v>
       </c>
       <c r="F2" s="3">
         <v>1</v>
@@ -74380,7 +74392,7 @@
         <v>1198</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F3" s="3">
         <v>1</v>
@@ -74412,7 +74424,7 @@
         <v>1199</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F4" s="12">
         <v>3</v>
@@ -74444,7 +74456,7 @@
         <v>1200</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F5" s="3">
         <v>3</v>
@@ -74476,7 +74488,7 @@
         <v>1201</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F6" s="3">
         <v>1</v>
@@ -74508,7 +74520,7 @@
         <v>1156</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F7" s="3">
         <v>1</v>
@@ -74543,7 +74555,7 @@
         <v>1202</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F8" s="3">
         <v>1</v>
@@ -74578,7 +74590,7 @@
         <v>1203</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F9" s="10">
         <v>1</v>
@@ -74613,7 +74625,7 @@
         <v>1437</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
@@ -74648,7 +74660,7 @@
         <v>1193</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F11" s="10">
         <v>1</v>
@@ -74680,7 +74692,7 @@
         <v>1160</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F12" s="3">
         <v>2</v>
@@ -74715,7 +74727,7 @@
         <v>1204</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F13" s="3">
         <v>1</v>
@@ -74750,7 +74762,7 @@
         <v>1157</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F14" s="3">
         <v>1</v>
@@ -74785,7 +74797,7 @@
         <v>1155</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F15" s="3">
         <v>1</v>
@@ -74817,7 +74829,7 @@
         <v>1158</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F16" s="3">
         <v>2</v>
@@ -74852,7 +74864,7 @@
         <v>1205</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F17" s="3">
         <v>1</v>
@@ -74887,7 +74899,7 @@
         <v>1208</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F18" s="3">
         <v>1</v>
@@ -74922,7 +74934,7 @@
         <v>1194</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F19" s="10">
         <v>1</v>
@@ -74954,7 +74966,7 @@
         <v>1154</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F20" s="3">
         <v>2</v>
@@ -74986,7 +74998,7 @@
         <v>1196</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F21" s="10">
         <v>1</v>
@@ -75018,7 +75030,7 @@
         <v>1209</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F22" s="10">
         <v>1</v>
@@ -75053,7 +75065,7 @@
         <v>1159</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F23" s="3">
         <v>1</v>
@@ -75088,7 +75100,7 @@
         <v>1153</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F24" s="3">
         <v>2</v>
@@ -75120,7 +75132,7 @@
         <v>1206</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F25" s="3">
         <v>1</v>
@@ -75155,7 +75167,7 @@
         <v>1195</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F26" s="10">
         <v>1</v>
@@ -75190,7 +75202,7 @@
         <v>1207</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F27" s="3">
         <v>1</v>
@@ -75225,7 +75237,7 @@
         <v>1210</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F28" s="10">
         <v>2</v>
@@ -75257,7 +75269,7 @@
         <v>1211</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F29" s="10">
         <v>1</v>
@@ -75292,7 +75304,7 @@
         <v>3110</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F30" s="3">
         <v>1</v>
@@ -75327,7 +75339,7 @@
         <v>3112</v>
       </c>
       <c r="E31" s="26" t="s">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="F31" s="3">
         <v>1</v>
@@ -75347,12 +75359,6 @@
       <c r="K31" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="E32" s="11"/>
-    </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.45">
-      <c r="E33" s="11"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:K33">
@@ -76124,7 +76130,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -76136,7 +76142,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>4281</v>
       </c>
       <c r="C1" s="19"/>
@@ -76147,7 +76153,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="27" t="s">
         <v>4278</v>
       </c>
     </row>
@@ -76156,7 +76162,7 @@
         <v>4279</v>
       </c>
       <c r="B5" t="s">
-        <v>4310</v>
+        <v>4307</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
@@ -76164,7 +76170,7 @@
         <v>4280</v>
       </c>
       <c r="B6" t="s">
-        <v>4309</v>
+        <v>4306</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
@@ -76172,7 +76178,7 @@
         <v>4283</v>
       </c>
       <c r="B7" t="s">
-        <v>4314</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
@@ -76180,27 +76186,27 @@
         <v>4284</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>4311</v>
+        <v>4308</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>4289</v>
+        <v>4286</v>
       </c>
       <c r="B9" t="s">
-        <v>4312</v>
+        <v>4309</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="19" t="s">
-        <v>4296</v>
+        <v>4293</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>4313</v>
+        <v>4310</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="27" t="s">
         <v>4285</v>
       </c>
     </row>
@@ -76209,13 +76215,13 @@
         <v>78</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>1145</v>
+        <v>4316</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>1146</v>
+        <v>4317</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>1151</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
@@ -76223,10 +76229,10 @@
         <v>44</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>4298</v>
+        <v>4295</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="D14" s="20">
         <v>2</v>
@@ -76237,7 +76243,7 @@
         <v>3914</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="20">
@@ -76249,7 +76255,7 @@
         <v>46</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>4300</v>
+        <v>4297</v>
       </c>
       <c r="C16" s="20"/>
       <c r="D16" s="20">
@@ -76276,7 +76282,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="D18" s="20">
         <v>2</v>
@@ -76287,7 +76293,7 @@
         <v>51</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>4301</v>
+        <v>4298</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="25">
@@ -76299,10 +76305,10 @@
         <v>3915</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>4302</v>
+        <v>4299</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>4299</v>
+        <v>4296</v>
       </c>
       <c r="D20" s="20">
         <v>2</v>
@@ -76325,7 +76331,7 @@
         <v>3917</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>4302</v>
+        <v>4299</v>
       </c>
       <c r="C22" s="20"/>
       <c r="D22" s="20">
@@ -76338,7 +76344,7 @@
       </c>
       <c r="B23" s="25"/>
       <c r="C23" s="20" t="s">
-        <v>4300</v>
+        <v>4297</v>
       </c>
       <c r="D23" s="20">
         <v>2</v>
@@ -76346,10 +76352,10 @@
     </row>
     <row r="24" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A24" s="21" t="s">
-        <v>4297</v>
+        <v>4294</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>4303</v>
+        <v>4300</v>
       </c>
       <c r="C24" s="20"/>
       <c r="D24" s="20">
@@ -76358,47 +76364,47 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="21" t="s">
-        <v>4286</v>
+        <v>4318</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="21" t="s">
-        <v>4287</v>
+        <v>4319</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="21" t="s">
-        <v>4288</v>
+        <v>4320</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A30" s="28" t="s">
-        <v>4290</v>
+      <c r="A30" s="27" t="s">
+        <v>4287</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="21" t="s">
-        <v>4291</v>
+        <v>4288</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="21" t="s">
-        <v>4292</v>
+        <v>4289</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" s="21" t="s">
-        <v>4295</v>
+        <v>4292</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" s="21" t="s">
-        <v>4293</v>
+        <v>4290</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" s="21" t="s">
-        <v>4294</v>
+        <v>4291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Converted ccw_lookup years to months
</commit_message>
<xml_diff>
--- a/claims_data/ccw_lookup.xlsx
+++ b/claims_data/ccw_lookup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kc1-my.sharepoint.com/personal/alastair_matheson_kingcounty_gov/Documents/github/reference-data/claims_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="425" documentId="11_9A33B9A22B7DCD35061FD0B4DF8B81B7DEB0F1C7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD55399E-1D95-488B-848D-64E6BD20C035}"/>
+  <xr:revisionPtr revIDLastSave="439" documentId="11_9A33B9A22B7DCD35061FD0B4DF8B81B7DEB0F1C7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01E90AA2-E0E1-4E32-A6C8-300271CB64ED}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="label" sheetId="4" state="hidden" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9129" uniqueCount="4315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9129" uniqueCount="4316">
   <si>
     <t>Acquired Hypothyrodism</t>
   </si>
@@ -13017,6 +13017,9 @@
   </si>
   <si>
     <t>condition_type = if all claims type only need 1 visit (=1) or some claim types need 2 visits (=2) in lookback period. Used to set up SQL code in claim_ccw function (https://github.com/PHSKC-APDE/claims_data/blob/main/claims_db/db_loader/scripts_general/claim_ccw.R).</t>
+  </si>
+  <si>
+    <t>lookback_months</t>
   </si>
 </sst>
 </file>
@@ -73070,8 +73073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D624538-775A-4896-8368-5AB97255472E}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:J1048576"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -73081,7 +73084,7 @@
     <col min="3" max="3" width="49.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" style="3" customWidth="1"/>
     <col min="5" max="5" width="15.265625" style="26" customWidth="1"/>
-    <col min="6" max="6" width="11.1328125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.265625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.86328125" style="14" customWidth="1"/>
     <col min="8" max="8" width="70.265625" style="4" customWidth="1"/>
     <col min="9" max="9" width="25.86328125" style="9" customWidth="1"/>
@@ -73106,7 +73109,7 @@
         <v>4307</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>37</v>
+        <v>4315</v>
       </c>
       <c r="G1" s="15" t="s">
         <v>4308</v>
@@ -73141,7 +73144,7 @@
         <v>4264</v>
       </c>
       <c r="F2" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>38</v>
@@ -73176,7 +73179,7 @@
         <v>4264</v>
       </c>
       <c r="F3" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>38</v>
@@ -73208,7 +73211,7 @@
         <v>4264</v>
       </c>
       <c r="F4" s="12">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G4" s="17" t="s">
         <v>38</v>
@@ -73243,7 +73246,7 @@
         <v>4298</v>
       </c>
       <c r="F5" s="3">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>38</v>
@@ -73275,7 +73278,7 @@
         <v>4264</v>
       </c>
       <c r="F6" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>38</v>
@@ -73310,7 +73313,7 @@
         <v>4264</v>
       </c>
       <c r="F7" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G7" s="14" t="s">
         <v>38</v>
@@ -73345,7 +73348,7 @@
         <v>4264</v>
       </c>
       <c r="F8" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G8" s="14" t="s">
         <v>38</v>
@@ -73380,7 +73383,7 @@
         <v>4264</v>
       </c>
       <c r="F9" s="10">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G9" s="14" t="s">
         <v>38</v>
@@ -73415,7 +73418,7 @@
         <v>4264</v>
       </c>
       <c r="F10" s="10">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G10" s="14" t="s">
         <v>38</v>
@@ -73450,7 +73453,7 @@
         <v>4264</v>
       </c>
       <c r="F11" s="10">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G11" s="14" t="s">
         <v>38</v>
@@ -73482,7 +73485,7 @@
         <v>4264</v>
       </c>
       <c r="F12" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G12" s="14" t="s">
         <v>38</v>
@@ -73517,7 +73520,7 @@
         <v>4264</v>
       </c>
       <c r="F13" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G13" s="14" t="s">
         <v>38</v>
@@ -73552,7 +73555,7 @@
         <v>4264</v>
       </c>
       <c r="F14" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G14" s="14" t="s">
         <v>38</v>
@@ -73587,7 +73590,7 @@
         <v>4264</v>
       </c>
       <c r="F15" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G15" s="14" t="s">
         <v>38</v>
@@ -73622,7 +73625,7 @@
         <v>4264</v>
       </c>
       <c r="F16" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G16" s="14" t="s">
         <v>38</v>
@@ -73657,7 +73660,7 @@
         <v>4264</v>
       </c>
       <c r="F17" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G17" s="14" t="s">
         <v>38</v>
@@ -73692,7 +73695,7 @@
         <v>4264</v>
       </c>
       <c r="F18" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G18" s="14" t="s">
         <v>38</v>
@@ -73727,7 +73730,7 @@
         <v>4264</v>
       </c>
       <c r="F19" s="10">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G19" s="14" t="s">
         <v>38</v>
@@ -73759,7 +73762,7 @@
         <v>4264</v>
       </c>
       <c r="F20" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G20" s="14" t="s">
         <v>38</v>
@@ -73794,7 +73797,7 @@
         <v>4264</v>
       </c>
       <c r="F21" s="10">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G21" s="14" t="s">
         <v>38</v>
@@ -73827,7 +73830,7 @@
         <v>4264</v>
       </c>
       <c r="F22" s="10">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G22" s="14" t="s">
         <v>38</v>
@@ -73862,7 +73865,7 @@
         <v>4264</v>
       </c>
       <c r="F23" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G23" s="14" t="s">
         <v>38</v>
@@ -73897,7 +73900,7 @@
         <v>4264</v>
       </c>
       <c r="F24" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G24" s="14" t="s">
         <v>38</v>
@@ -73932,7 +73935,7 @@
         <v>4264</v>
       </c>
       <c r="F25" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G25" s="14" t="s">
         <v>38</v>
@@ -73967,7 +73970,7 @@
         <v>4264</v>
       </c>
       <c r="F26" s="10">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G26" s="14" t="s">
         <v>38</v>
@@ -74002,7 +74005,7 @@
         <v>4264</v>
       </c>
       <c r="F27" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G27" s="14" t="s">
         <v>38</v>
@@ -74037,7 +74040,7 @@
         <v>4264</v>
       </c>
       <c r="F28" s="10">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G28" s="16" t="s">
         <v>38</v>
@@ -74072,7 +74075,7 @@
         <v>4264</v>
       </c>
       <c r="F29" s="10">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G29" s="16" t="s">
         <v>38</v>
@@ -74105,7 +74108,7 @@
         <v>4264</v>
       </c>
       <c r="F30" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G30" s="14" t="s">
         <v>38</v>
@@ -74138,7 +74141,7 @@
         <v>4264</v>
       </c>
       <c r="F31" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G31" s="14" t="s">
         <v>38</v>
@@ -74173,7 +74176,7 @@
         <v>4264</v>
       </c>
       <c r="F32" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G32" s="26" t="s">
         <v>38</v>
@@ -74208,7 +74211,7 @@
         <v>4264</v>
       </c>
       <c r="F33" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G33" s="26" t="s">
         <v>38</v>
@@ -74243,7 +74246,7 @@
         <v>4264</v>
       </c>
       <c r="F34" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G34" s="26" t="s">
         <v>38</v>
@@ -74271,8 +74274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -74282,7 +74285,7 @@
     <col min="3" max="3" width="49.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" style="3" customWidth="1"/>
     <col min="5" max="5" width="15.265625" style="26" customWidth="1"/>
-    <col min="6" max="6" width="11.1328125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.265625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.86328125" style="14" customWidth="1"/>
     <col min="8" max="8" width="70.265625" style="4" customWidth="1"/>
     <col min="9" max="9" width="25.86328125" style="9" customWidth="1"/>
@@ -74307,7 +74310,7 @@
         <v>4307</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>37</v>
+        <v>4315</v>
       </c>
       <c r="G1" s="15" t="s">
         <v>4308</v>
@@ -74342,7 +74345,7 @@
         <v>4298</v>
       </c>
       <c r="F2" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>38</v>
@@ -74377,7 +74380,7 @@
         <v>4298</v>
       </c>
       <c r="F3" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>4293</v>
@@ -74409,7 +74412,7 @@
         <v>4298</v>
       </c>
       <c r="F4" s="12">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="G4" s="17" t="s">
         <v>38</v>
@@ -74441,7 +74444,7 @@
         <v>4298</v>
       </c>
       <c r="F5" s="3">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>38</v>
@@ -74473,7 +74476,7 @@
         <v>4298</v>
       </c>
       <c r="F6" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>38</v>
@@ -74505,7 +74508,7 @@
         <v>4298</v>
       </c>
       <c r="F7" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G7" s="14" t="s">
         <v>38</v>
@@ -74540,7 +74543,7 @@
         <v>4298</v>
       </c>
       <c r="F8" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G8" s="14" t="s">
         <v>4293</v>
@@ -74575,7 +74578,7 @@
         <v>4298</v>
       </c>
       <c r="F9" s="10">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G9" s="14" t="s">
         <v>38</v>
@@ -74610,7 +74613,7 @@
         <v>4298</v>
       </c>
       <c r="F10" s="10">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G10" s="14" t="s">
         <v>38</v>
@@ -74645,7 +74648,7 @@
         <v>4298</v>
       </c>
       <c r="F11" s="10">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G11" s="14" t="s">
         <v>3907</v>
@@ -74677,7 +74680,7 @@
         <v>4298</v>
       </c>
       <c r="F12" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G12" s="14" t="s">
         <v>38</v>
@@ -74712,7 +74715,7 @@
         <v>4298</v>
       </c>
       <c r="F13" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G13" s="14" t="s">
         <v>38</v>
@@ -74747,7 +74750,7 @@
         <v>4298</v>
       </c>
       <c r="F14" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G14" s="14" t="s">
         <v>38</v>
@@ -74782,7 +74785,7 @@
         <v>4298</v>
       </c>
       <c r="F15" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G15" s="14" t="s">
         <v>38</v>
@@ -74814,7 +74817,7 @@
         <v>4298</v>
       </c>
       <c r="F16" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G16" s="14" t="s">
         <v>38</v>
@@ -74849,7 +74852,7 @@
         <v>4298</v>
       </c>
       <c r="F17" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G17" s="14" t="s">
         <v>38</v>
@@ -74884,7 +74887,7 @@
         <v>4298</v>
       </c>
       <c r="F18" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G18" s="14" t="s">
         <v>38</v>
@@ -74919,7 +74922,7 @@
         <v>4298</v>
       </c>
       <c r="F19" s="10">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G19" s="14" t="s">
         <v>3907</v>
@@ -74951,7 +74954,7 @@
         <v>4298</v>
       </c>
       <c r="F20" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G20" s="14" t="s">
         <v>38</v>
@@ -74983,7 +74986,7 @@
         <v>4298</v>
       </c>
       <c r="F21" s="10">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G21" s="14" t="s">
         <v>38</v>
@@ -75015,7 +75018,7 @@
         <v>4298</v>
       </c>
       <c r="F22" s="10">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G22" s="14" t="s">
         <v>38</v>
@@ -75050,7 +75053,7 @@
         <v>4298</v>
       </c>
       <c r="F23" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G23" s="14" t="s">
         <v>38</v>
@@ -75085,7 +75088,7 @@
         <v>4298</v>
       </c>
       <c r="F24" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G24" s="14" t="s">
         <v>38</v>
@@ -75117,7 +75120,7 @@
         <v>4298</v>
       </c>
       <c r="F25" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G25" s="14" t="s">
         <v>38</v>
@@ -75152,7 +75155,7 @@
         <v>4298</v>
       </c>
       <c r="F26" s="10">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G26" s="14" t="s">
         <v>38</v>
@@ -75187,7 +75190,7 @@
         <v>4298</v>
       </c>
       <c r="F27" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G27" s="14" t="s">
         <v>38</v>
@@ -75222,7 +75225,7 @@
         <v>4298</v>
       </c>
       <c r="F28" s="10">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G28" s="16" t="s">
         <v>38</v>
@@ -75254,7 +75257,7 @@
         <v>4298</v>
       </c>
       <c r="F29" s="10">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G29" s="16" t="s">
         <v>38</v>
@@ -75289,7 +75292,7 @@
         <v>4298</v>
       </c>
       <c r="F30" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G30" s="14" t="s">
         <v>38</v>
@@ -75324,7 +75327,7 @@
         <v>4298</v>
       </c>
       <c r="F31" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G31" s="14">
         <v>1</v>
@@ -76405,12 +76408,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010098C197DC67C0514EB308983AEF32E983" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a506a90b446ec8f6ca9341c1992a61de">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d55fa3f-3c18-425b-9faa-377f011f8097" xmlns:ns3="39d3cee1-f650-41e8-9a2f-4357c6682977" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="68eb73591874d7b6cee55945c0a8d5bf" ns2:_="" ns3:_="">
     <xsd:import namespace="3d55fa3f-3c18-425b-9faa-377f011f8097"/>
@@ -76587,6 +76584,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76AD4B54-6DC2-4D8C-86CA-5908AE6EF015}">
   <ds:schemaRefs>
@@ -76596,23 +76599,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC2EEFE0-2F39-4B6B-9A9A-7092F0DE0B00}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="3d55fa3f-3c18-425b-9faa-377f011f8097"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="39d3cee1-f650-41e8-9a2f-4357c6682977"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A61351A-2F7F-48FB-A782-AE9A92A10B40}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -76629,4 +76615,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC2EEFE0-2F39-4B6B-9A9A-7092F0DE0B00}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="3d55fa3f-3c18-425b-9faa-377f011f8097"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="39d3cee1-f650-41e8-9a2f-4357c6682977"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Additional tweaks to claim CCW table
</commit_message>
<xml_diff>
--- a/claims_data/ccw_lookup.xlsx
+++ b/claims_data/ccw_lookup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kc1-my.sharepoint.com/personal/alastair_matheson_kingcounty_gov/Documents/github/reference-data/claims_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="439" documentId="11_9A33B9A22B7DCD35061FD0B4DF8B81B7DEB0F1C7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01E90AA2-E0E1-4E32-A6C8-300271CB64ED}"/>
+  <xr:revisionPtr revIDLastSave="467" documentId="11_9A33B9A22B7DCD35061FD0B4DF8B81B7DEB0F1C7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8B97DAB-9558-454F-B650-E427D982F649}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73074,7 +73074,7 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -74275,7 +74275,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -76408,6 +76408,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010098C197DC67C0514EB308983AEF32E983" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a506a90b446ec8f6ca9341c1992a61de">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d55fa3f-3c18-425b-9faa-377f011f8097" xmlns:ns3="39d3cee1-f650-41e8-9a2f-4357c6682977" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="68eb73591874d7b6cee55945c0a8d5bf" ns2:_="" ns3:_="">
     <xsd:import namespace="3d55fa3f-3c18-425b-9faa-377f011f8097"/>
@@ -76584,12 +76590,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76AD4B54-6DC2-4D8C-86CA-5908AE6EF015}">
   <ds:schemaRefs>
@@ -76599,6 +76599,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC2EEFE0-2F39-4B6B-9A9A-7092F0DE0B00}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="3d55fa3f-3c18-425b-9faa-377f011f8097"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="39d3cee1-f650-41e8-9a2f-4357c6682977"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A61351A-2F7F-48FB-A782-AE9A92A10B40}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -76615,21 +76632,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC2EEFE0-2F39-4B6B-9A9A-7092F0DE0B00}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="3d55fa3f-3c18-425b-9faa-377f011f8097"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="39d3cee1-f650-41e8-9a2f-4357c6682977"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Using new CCW lookback, dx code, claim types for all years
</commit_message>
<xml_diff>
--- a/claims_data/ccw_lookup.xlsx
+++ b/claims_data/ccw_lookup.xlsx
@@ -8,27 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kc1-my.sharepoint.com/personal/alastair_matheson_kingcounty_gov/Documents/github/reference-data/claims_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="467" documentId="11_9A33B9A22B7DCD35061FD0B4DF8B81B7DEB0F1C7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8B97DAB-9558-454F-B650-E427D982F649}"/>
+  <xr:revisionPtr revIDLastSave="492" documentId="11_9A33B9A22B7DCD35061FD0B4DF8B81B7DEB0F1C7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E38603D-BFFB-458B-8380-E9FB2C5F8BA7}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="label" sheetId="4" state="hidden" r:id="rId1"/>
-    <sheet name="ccw17_xx" sheetId="16" r:id="rId2"/>
-    <sheet name="ccw99_16" sheetId="11" r:id="rId3"/>
-    <sheet name="ccw_definitions_kc_17_xx" sheetId="17" r:id="rId4"/>
-    <sheet name="ccw_definitions_kc_99_16" sheetId="15" r:id="rId5"/>
-    <sheet name="ccw_definitions_p1" sheetId="12" r:id="rId6"/>
-    <sheet name="ccw_definitions_apcd" sheetId="13" r:id="rId7"/>
-    <sheet name="ccw_instructions" sheetId="18" r:id="rId8"/>
+    <sheet name="ccw_instructions" sheetId="18" r:id="rId2"/>
+    <sheet name="ccw17_xx" sheetId="16" r:id="rId3"/>
+    <sheet name="ccw99_16" sheetId="11" r:id="rId4"/>
+    <sheet name="ccw_definitions_kc_99_xx" sheetId="19" r:id="rId5"/>
+    <sheet name="ccw_definitions_kc_17_xx" sheetId="17" r:id="rId6"/>
+    <sheet name="ccw_definitions_kc_99_16" sheetId="15" r:id="rId7"/>
+    <sheet name="ccw_definitions_p1" sheetId="12" r:id="rId8"/>
+    <sheet name="ccw_definitions_apcd" sheetId="13" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">ccw_definitions_apcd!$A$1:$G$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ccw_definitions_kc_17_xx!$B$1:$K$30</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ccw_definitions_kc_99_16!$B$1:$K$31</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">ccw_definitions_p1!$A$1:$I$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ccw17_xx!$A$1:$D$2992</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ccw99_16!$A$1:$D$1211</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">ccw_definitions_apcd!$A$1:$G$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">ccw_definitions_kc_17_xx!$B$1:$K$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">ccw_definitions_kc_99_16!$B$1:$K$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ccw_definitions_kc_99_xx!$B$1:$K$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">ccw_definitions_p1!$A$1:$I$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ccw17_xx!$A$1:$D$2992</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ccw99_16!$A$1:$D$1211</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9129" uniqueCount="4316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9566" uniqueCount="4318">
   <si>
     <t>Acquired Hypothyrodism</t>
   </si>
@@ -12957,13 +12959,46 @@
     <t>Contains ICD-10-CM codes for each condition from the 30 CCW Chronic Conditions doc (claims &gt;= October 2016). Use this for making ref_dx_lookup tables.</t>
   </si>
   <si>
-    <t>Contains CCW code, description, lookback period, types of claims considered, and number of claims needed for each chronic condition. Derived from previous 27 CCW Chronic Conditions doc and applied to claims &lt; October 2016. Use this to make ref_ccw_lookup.</t>
-  </si>
-  <si>
     <t>Contains definitions for each chronic condition but using claim types specific to Provider1/Medicaid data. Outdated, use ccw_definitions_kc sheets.</t>
   </si>
   <si>
     <t>Contains definitions for each chronic condition but using claim and setting types specific to All Payer Claims Data. Outdated, use ccw_definitions_kc sheets.</t>
+  </si>
+  <si>
+    <t>ccw_icd_version</t>
+  </si>
+  <si>
+    <t>ccw_version</t>
+  </si>
+  <si>
+    <t>dx_fields</t>
+  </si>
+  <si>
+    <t>condition_type</t>
+  </si>
+  <si>
+    <t>claim_type_1</t>
+  </si>
+  <si>
+    <t>claim_type_2</t>
+  </si>
+  <si>
+    <t>claim_type_1 = types of claim that need 1 visit in the lookback period</t>
+  </si>
+  <si>
+    <t>claim_type_2 = types of claim that need 2 visits in the lookback period</t>
+  </si>
+  <si>
+    <t>condition_type = if all claims type only need 1 visit (=1) or some claim types need 2 visits (=2) in lookback period. Used to set up SQL code in claim_ccw function (https://github.com/PHSKC-APDE/claims_data/blob/main/claims_db/db_loader/scripts_general/claim_ccw.R).</t>
+  </si>
+  <si>
+    <t>lookback_months</t>
+  </si>
+  <si>
+    <t>ccw_definitions_kc_17_xx</t>
+  </si>
+  <si>
+    <t>Contains CCW code, description, lookback period, types of claims considered, and number of claims needed for each chronic condition. Derived from current 30 CCW Chronic Conditions doc and applied to all time periods (including those with ICD-9-CM codes). Use this to make ref_ccw_lookup.</t>
   </si>
   <si>
     <r>
@@ -12988,38 +13023,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, which covers ICD-9 and ICD-10 but is derived from the 27 CCW doc). Use this to make ref_ccw_lookup.</t>
+      <t>, which covers ICD-9 and ICD-10 but is derived from the 27 CCW doc). Outdated, use ccw_definitions_kc_99_xx to make ref_ccw_lookup.</t>
     </r>
   </si>
   <si>
-    <t>ccw_icd_version</t>
-  </si>
-  <si>
-    <t>ccw_version</t>
-  </si>
-  <si>
-    <t>dx_fields</t>
-  </si>
-  <si>
-    <t>condition_type</t>
-  </si>
-  <si>
-    <t>claim_type_1</t>
-  </si>
-  <si>
-    <t>claim_type_2</t>
-  </si>
-  <si>
-    <t>claim_type_1 = types of claim that need 1 visit in the lookback period</t>
-  </si>
-  <si>
-    <t>claim_type_2 = types of claim that need 2 visits in the lookback period</t>
-  </si>
-  <si>
-    <t>condition_type = if all claims type only need 1 visit (=1) or some claim types need 2 visits (=2) in lookback period. Used to set up SQL code in claim_ccw function (https://github.com/PHSKC-APDE/claims_data/blob/main/claims_db/db_loader/scripts_general/claim_ccw.R).</t>
-  </si>
-  <si>
-    <t>lookback_months</t>
+    <t>Contains CCW code, description, lookback period, types of claims considered, and number of claims needed for each chronic condition. Derived from previous 27 CCW Chronic Conditions doc and applied to claims &lt; October 2016. Outdated, use ccw_definitions_kc_99_xx to make ref_ccw_lookup.</t>
   </si>
 </sst>
 </file>
@@ -14183,6 +14191,302 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F3F6B6C-5426-41AC-9E1E-CFE1B1525272}">
+  <dimension ref="A1:D36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="65.73046875" customWidth="1"/>
+    <col min="2" max="2" width="11.86328125" customWidth="1"/>
+    <col min="3" max="3" width="12.59765625" customWidth="1"/>
+    <col min="4" max="4" width="13.86328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="27" t="s">
+        <v>4275</v>
+      </c>
+      <c r="C1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="19" t="s">
+        <v>4276</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" s="27" t="s">
+        <v>4272</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>4273</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>4274</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="19" t="s">
+        <v>4277</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>4315</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>4314</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4316</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" s="19" t="s">
+        <v>4278</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>4317</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>4280</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4302</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" s="19" t="s">
+        <v>4287</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>4303</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" s="27" t="s">
+        <v>4279</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>4308</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>4309</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>4307</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="D15" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="21" t="s">
+        <v>3908</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>4290</v>
+      </c>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>4291</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" s="21" t="s">
+        <v>3905</v>
+      </c>
+      <c r="B18" s="25">
+        <v>1</v>
+      </c>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" s="21" t="s">
+        <v>3906</v>
+      </c>
+      <c r="B19" s="25">
+        <v>1</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="D19" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>4292</v>
+      </c>
+      <c r="C20" s="20"/>
+      <c r="D20" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" s="21" t="s">
+        <v>3909</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>4293</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="D21" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22" s="21" t="s">
+        <v>3910</v>
+      </c>
+      <c r="B22" s="25">
+        <v>5</v>
+      </c>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" s="21" t="s">
+        <v>3911</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>4293</v>
+      </c>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" s="21" t="s">
+        <v>3912</v>
+      </c>
+      <c r="B24" s="25"/>
+      <c r="C24" s="20" t="s">
+        <v>4291</v>
+      </c>
+      <c r="D24" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="21" t="s">
+        <v>4288</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>4294</v>
+      </c>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" s="21" t="s">
+        <v>4310</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" s="21" t="s">
+        <v>4311</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29" s="21" t="s">
+        <v>4312</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31" s="27" t="s">
+        <v>4281</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32" s="21" t="s">
+        <v>4282</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A33" s="21" t="s">
+        <v>4283</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A34" s="21" t="s">
+        <v>4286</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A35" s="21" t="s">
+        <v>4284</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A36" s="21" t="s">
+        <v>4285</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D2B65D-303C-44A5-AECA-47B2694A297B}">
   <dimension ref="A1:D2992"/>
   <sheetViews>
@@ -56092,7 +56396,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D1211"/>
   <sheetViews>
@@ -73069,12 +73373,2237 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47AACAD2-3D50-4D3E-8D59-88E07F1DABAD}">
+  <dimension ref="A1:K64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="13.9296875" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.3984375" style="20" customWidth="1"/>
+    <col min="3" max="3" width="49.33203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" style="20" customWidth="1"/>
+    <col min="5" max="5" width="15.265625" style="26" customWidth="1"/>
+    <col min="6" max="6" width="15.265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.86328125" style="26" customWidth="1"/>
+    <col min="8" max="8" width="70.265625" style="21" customWidth="1"/>
+    <col min="9" max="9" width="25.86328125" style="25" customWidth="1"/>
+    <col min="10" max="10" width="15.59765625" style="20" customWidth="1"/>
+    <col min="11" max="11" width="15.265625" style="20" customWidth="1"/>
+    <col min="12" max="16384" width="9.06640625" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1" s="18" t="s">
+        <v>4304</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>1187</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>1188</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>4305</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>4313</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>4306</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>4308</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>4309</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>4307</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A2" s="19">
+        <v>10</v>
+      </c>
+      <c r="B2" s="20">
+        <v>1</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>4265</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>1193</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F2" s="20">
+        <v>24</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K2" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3" s="19">
+        <v>10</v>
+      </c>
+      <c r="B3" s="20">
+        <v>2</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>1174</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>1194</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F3" s="20">
+        <v>12</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>3905</v>
+      </c>
+      <c r="I3" s="25">
+        <v>1</v>
+      </c>
+      <c r="K3" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A4" s="19">
+        <v>10</v>
+      </c>
+      <c r="B4" s="20">
+        <v>3</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F4" s="12">
+        <v>24</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K4" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A5" s="19">
+        <v>10</v>
+      </c>
+      <c r="B5" s="20">
+        <v>4</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>1196</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>4298</v>
+      </c>
+      <c r="F5" s="20">
+        <v>36</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>4291</v>
+      </c>
+      <c r="K5" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A6" s="19">
+        <v>10</v>
+      </c>
+      <c r="B6" s="20">
+        <v>5</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>1197</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F6" s="20">
+        <v>24</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K6" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A7" s="19">
+        <v>10</v>
+      </c>
+      <c r="B7" s="20">
+        <v>6</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>1156</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F7" s="20">
+        <v>24</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K7" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A8" s="19">
+        <v>10</v>
+      </c>
+      <c r="B8" s="20">
+        <v>7</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>4268</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>1198</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F8" s="20">
+        <v>24</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K8" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A9" s="19">
+        <v>10</v>
+      </c>
+      <c r="B9" s="20">
+        <v>8</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>1178</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>1199</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F9" s="10">
+        <v>24</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K9" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A10" s="19">
+        <v>10</v>
+      </c>
+      <c r="B10" s="20">
+        <v>8.1</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>3104</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>1433</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F10" s="10">
+        <v>24</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K10" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A11" s="19">
+        <v>10</v>
+      </c>
+      <c r="B11" s="20">
+        <v>9</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>1189</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F11" s="10">
+        <v>12</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>3908</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K11" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A12" s="19">
+        <v>10</v>
+      </c>
+      <c r="B12" s="20">
+        <v>10</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>963</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F12" s="20">
+        <v>24</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K12" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A13" s="19">
+        <v>10</v>
+      </c>
+      <c r="B13" s="20">
+        <v>11</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>1183</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>1200</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F13" s="20">
+        <v>24</v>
+      </c>
+      <c r="G13" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>3909</v>
+      </c>
+      <c r="I13" s="25" t="s">
+        <v>4293</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K13" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A14" s="19">
+        <v>10</v>
+      </c>
+      <c r="B14" s="20">
+        <v>12</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>3913</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F14" s="20">
+        <v>24</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J14" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K14" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A15" s="19">
+        <v>10</v>
+      </c>
+      <c r="B15" s="20">
+        <v>13</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>4270</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>1155</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F15" s="20">
+        <v>24</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J15" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K15" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A16" s="19">
+        <v>10</v>
+      </c>
+      <c r="B16" s="20">
+        <v>14</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>1158</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F16" s="20">
+        <v>24</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J16" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K16" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A17" s="19">
+        <v>10</v>
+      </c>
+      <c r="B17" s="20">
+        <v>15</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>1201</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F17" s="20">
+        <v>24</v>
+      </c>
+      <c r="G17" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="21" t="s">
+        <v>3909</v>
+      </c>
+      <c r="I17" s="25" t="s">
+        <v>4293</v>
+      </c>
+      <c r="J17" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K17" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A18" s="19">
+        <v>10</v>
+      </c>
+      <c r="B18" s="20">
+        <v>16</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>1182</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>1204</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F18" s="20">
+        <v>24</v>
+      </c>
+      <c r="G18" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" s="21" t="s">
+        <v>3909</v>
+      </c>
+      <c r="I18" s="25" t="s">
+        <v>4293</v>
+      </c>
+      <c r="J18" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K18" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A19" s="19">
+        <v>10</v>
+      </c>
+      <c r="B19" s="20">
+        <v>17</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>1190</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F19" s="10">
+        <v>24</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H19" s="21" t="s">
+        <v>3908</v>
+      </c>
+      <c r="I19" s="25" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K19" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A20" s="19">
+        <v>10</v>
+      </c>
+      <c r="B20" s="20">
+        <v>18</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>4271</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F20" s="20">
+        <v>24</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I20" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J20" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K20" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A21" s="19">
+        <v>10</v>
+      </c>
+      <c r="B21" s="20">
+        <v>19</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>1179</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F21" s="10">
+        <v>12</v>
+      </c>
+      <c r="G21" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H21" s="21" t="s">
+        <v>4288</v>
+      </c>
+      <c r="I21" s="25" t="s">
+        <v>4294</v>
+      </c>
+      <c r="K21" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A22" s="19">
+        <v>10</v>
+      </c>
+      <c r="B22" s="20">
+        <v>20</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>1205</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F22" s="10">
+        <v>24</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I22" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J22" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K22" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A23" s="19">
+        <v>10</v>
+      </c>
+      <c r="B23" s="20">
+        <v>21</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>1159</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F23" s="20">
+        <v>24</v>
+      </c>
+      <c r="G23" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J23" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K23" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A24" s="19">
+        <v>10</v>
+      </c>
+      <c r="B24" s="20">
+        <v>22</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>656</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>1153</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F24" s="20">
+        <v>24</v>
+      </c>
+      <c r="G24" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I24" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J24" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K24" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A25" s="19">
+        <v>10</v>
+      </c>
+      <c r="B25" s="20">
+        <v>23</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>1185</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>1202</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F25" s="20">
+        <v>24</v>
+      </c>
+      <c r="G25" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H25" s="21" t="s">
+        <v>3909</v>
+      </c>
+      <c r="I25" s="25" t="s">
+        <v>4293</v>
+      </c>
+      <c r="J25" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K25" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A26" s="19">
+        <v>10</v>
+      </c>
+      <c r="B26" s="20">
+        <v>24</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>4296</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>1191</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F26" s="10">
+        <v>24</v>
+      </c>
+      <c r="G26" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H26" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I26" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J26" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K26" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A27" s="19">
+        <v>10</v>
+      </c>
+      <c r="B27" s="20">
+        <v>25</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>1184</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>1203</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F27" s="20">
+        <v>24</v>
+      </c>
+      <c r="G27" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H27" s="21" t="s">
+        <v>3909</v>
+      </c>
+      <c r="I27" s="25" t="s">
+        <v>4293</v>
+      </c>
+      <c r="J27" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K27" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A28" s="19">
+        <v>10</v>
+      </c>
+      <c r="B28" s="20">
+        <v>26</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>1180</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>1206</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F28" s="10">
+        <v>24</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H28" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I28" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J28" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K28" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A29" s="19">
+        <v>10</v>
+      </c>
+      <c r="B29" s="20">
+        <v>27</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E29" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F29" s="10">
+        <v>12</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H29" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="I29" s="20" t="s">
+        <v>4292</v>
+      </c>
+      <c r="K29" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A30" s="19">
+        <v>10</v>
+      </c>
+      <c r="B30" s="20">
+        <v>27.1</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>3105</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>3106</v>
+      </c>
+      <c r="E30" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F30" s="20">
+        <v>12</v>
+      </c>
+      <c r="G30" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H30" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="I30" s="20" t="s">
+        <v>4292</v>
+      </c>
+      <c r="K30" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A31" s="19">
+        <v>10</v>
+      </c>
+      <c r="B31" s="20">
+        <v>28</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>4269</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>3974</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F31" s="20">
+        <v>24</v>
+      </c>
+      <c r="G31" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H31" s="21" t="s">
+        <v>3909</v>
+      </c>
+      <c r="I31" s="25" t="s">
+        <v>4293</v>
+      </c>
+      <c r="J31" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K31" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="19">
+        <v>10</v>
+      </c>
+      <c r="B32" s="20">
+        <v>29</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>4295</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>4040</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F32" s="20">
+        <v>24</v>
+      </c>
+      <c r="G32" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H32" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I32" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J32" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K32" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A33" s="19">
+        <v>10</v>
+      </c>
+      <c r="B33" s="20">
+        <v>30</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>4297</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>4083</v>
+      </c>
+      <c r="E33" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F33" s="20">
+        <v>24</v>
+      </c>
+      <c r="G33" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H33" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I33" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J33" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K33" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A34" s="19">
+        <v>10</v>
+      </c>
+      <c r="B34" s="20">
+        <v>31</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>4299</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>4182</v>
+      </c>
+      <c r="E34" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F34" s="20">
+        <v>12</v>
+      </c>
+      <c r="G34" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H34" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I34" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J34" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K34" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A35" s="19">
+        <v>9</v>
+      </c>
+      <c r="B35" s="20">
+        <v>1</v>
+      </c>
+      <c r="C35" s="21" t="s">
+        <v>4265</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>1193</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F35" s="20">
+        <v>24</v>
+      </c>
+      <c r="G35" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H35" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I35" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J35" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K35" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A36" s="19">
+        <v>9</v>
+      </c>
+      <c r="B36" s="20">
+        <v>2</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>1174</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>1194</v>
+      </c>
+      <c r="E36" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F36" s="20">
+        <v>12</v>
+      </c>
+      <c r="G36" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H36" s="21" t="s">
+        <v>3905</v>
+      </c>
+      <c r="I36" s="25">
+        <v>1</v>
+      </c>
+      <c r="K36" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A37" s="19">
+        <v>9</v>
+      </c>
+      <c r="B37" s="20">
+        <v>3</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E37" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F37" s="12">
+        <v>24</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H37" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I37" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J37" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K37" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A38" s="19">
+        <v>9</v>
+      </c>
+      <c r="B38" s="20">
+        <v>4</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>1196</v>
+      </c>
+      <c r="E38" s="26" t="s">
+        <v>4298</v>
+      </c>
+      <c r="F38" s="20">
+        <v>36</v>
+      </c>
+      <c r="G38" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H38" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="I38" s="20" t="s">
+        <v>4291</v>
+      </c>
+      <c r="K38" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A39" s="19">
+        <v>9</v>
+      </c>
+      <c r="B39" s="20">
+        <v>5</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>1197</v>
+      </c>
+      <c r="E39" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F39" s="20">
+        <v>24</v>
+      </c>
+      <c r="G39" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H39" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I39" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J39" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K39" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A40" s="19">
+        <v>9</v>
+      </c>
+      <c r="B40" s="20">
+        <v>6</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>1156</v>
+      </c>
+      <c r="E40" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F40" s="20">
+        <v>24</v>
+      </c>
+      <c r="G40" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H40" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I40" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J40" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K40" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A41" s="19">
+        <v>9</v>
+      </c>
+      <c r="B41" s="20">
+        <v>7</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>4268</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>1198</v>
+      </c>
+      <c r="E41" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F41" s="20">
+        <v>24</v>
+      </c>
+      <c r="G41" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H41" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I41" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J41" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K41" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A42" s="19">
+        <v>9</v>
+      </c>
+      <c r="B42" s="20">
+        <v>8</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>1178</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>1199</v>
+      </c>
+      <c r="E42" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F42" s="10">
+        <v>24</v>
+      </c>
+      <c r="G42" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H42" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I42" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J42" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K42" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A43" s="19">
+        <v>9</v>
+      </c>
+      <c r="B43" s="20">
+        <v>8.1</v>
+      </c>
+      <c r="C43" s="21" t="s">
+        <v>3104</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>1433</v>
+      </c>
+      <c r="E43" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F43" s="10">
+        <v>24</v>
+      </c>
+      <c r="G43" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H43" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I43" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J43" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K43" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A44" s="19">
+        <v>9</v>
+      </c>
+      <c r="B44" s="20">
+        <v>9</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>1189</v>
+      </c>
+      <c r="E44" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F44" s="10">
+        <v>12</v>
+      </c>
+      <c r="G44" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H44" s="21" t="s">
+        <v>3908</v>
+      </c>
+      <c r="I44" s="25" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K44" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A45" s="19">
+        <v>9</v>
+      </c>
+      <c r="B45" s="20">
+        <v>10</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>963</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E45" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F45" s="20">
+        <v>24</v>
+      </c>
+      <c r="G45" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H45" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I45" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J45" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K45" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A46" s="19">
+        <v>9</v>
+      </c>
+      <c r="B46" s="20">
+        <v>11</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>1183</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>1200</v>
+      </c>
+      <c r="E46" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F46" s="20">
+        <v>24</v>
+      </c>
+      <c r="G46" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H46" s="21" t="s">
+        <v>3909</v>
+      </c>
+      <c r="I46" s="25" t="s">
+        <v>4293</v>
+      </c>
+      <c r="J46" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K46" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A47" s="19">
+        <v>9</v>
+      </c>
+      <c r="B47" s="20">
+        <v>12</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>3913</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E47" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F47" s="20">
+        <v>24</v>
+      </c>
+      <c r="G47" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H47" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I47" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J47" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K47" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A48" s="19">
+        <v>9</v>
+      </c>
+      <c r="B48" s="20">
+        <v>13</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>4270</v>
+      </c>
+      <c r="D48" s="20" t="s">
+        <v>1155</v>
+      </c>
+      <c r="E48" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F48" s="20">
+        <v>24</v>
+      </c>
+      <c r="G48" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H48" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I48" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J48" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K48" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A49" s="19">
+        <v>9</v>
+      </c>
+      <c r="B49" s="20">
+        <v>14</v>
+      </c>
+      <c r="C49" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" s="20" t="s">
+        <v>1158</v>
+      </c>
+      <c r="E49" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F49" s="20">
+        <v>24</v>
+      </c>
+      <c r="G49" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H49" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I49" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J49" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K49" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A50" s="19">
+        <v>9</v>
+      </c>
+      <c r="B50" s="20">
+        <v>15</v>
+      </c>
+      <c r="C50" s="21" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D50" s="20" t="s">
+        <v>1201</v>
+      </c>
+      <c r="E50" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F50" s="20">
+        <v>24</v>
+      </c>
+      <c r="G50" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H50" s="21" t="s">
+        <v>3909</v>
+      </c>
+      <c r="I50" s="25" t="s">
+        <v>4293</v>
+      </c>
+      <c r="J50" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K50" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A51" s="19">
+        <v>9</v>
+      </c>
+      <c r="B51" s="20">
+        <v>16</v>
+      </c>
+      <c r="C51" s="21" t="s">
+        <v>1182</v>
+      </c>
+      <c r="D51" s="20" t="s">
+        <v>1204</v>
+      </c>
+      <c r="E51" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F51" s="20">
+        <v>24</v>
+      </c>
+      <c r="G51" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H51" s="21" t="s">
+        <v>3909</v>
+      </c>
+      <c r="I51" s="25" t="s">
+        <v>4293</v>
+      </c>
+      <c r="J51" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K51" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A52" s="19">
+        <v>9</v>
+      </c>
+      <c r="B52" s="20">
+        <v>17</v>
+      </c>
+      <c r="C52" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="20" t="s">
+        <v>1190</v>
+      </c>
+      <c r="E52" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F52" s="10">
+        <v>24</v>
+      </c>
+      <c r="G52" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H52" s="21" t="s">
+        <v>3908</v>
+      </c>
+      <c r="I52" s="25" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K52" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A53" s="19">
+        <v>9</v>
+      </c>
+      <c r="B53" s="20">
+        <v>18</v>
+      </c>
+      <c r="C53" s="21" t="s">
+        <v>4271</v>
+      </c>
+      <c r="D53" s="20" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E53" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F53" s="20">
+        <v>24</v>
+      </c>
+      <c r="G53" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H53" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I53" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J53" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K53" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A54" s="19">
+        <v>9</v>
+      </c>
+      <c r="B54" s="20">
+        <v>19</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>1179</v>
+      </c>
+      <c r="D54" s="20" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E54" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F54" s="10">
+        <v>12</v>
+      </c>
+      <c r="G54" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H54" s="21" t="s">
+        <v>4288</v>
+      </c>
+      <c r="I54" s="25" t="s">
+        <v>4294</v>
+      </c>
+      <c r="K54" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A55" s="19">
+        <v>9</v>
+      </c>
+      <c r="B55" s="20">
+        <v>20</v>
+      </c>
+      <c r="C55" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" s="20" t="s">
+        <v>1205</v>
+      </c>
+      <c r="E55" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F55" s="10">
+        <v>24</v>
+      </c>
+      <c r="G55" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H55" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I55" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J55" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K55" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A56" s="19">
+        <v>9</v>
+      </c>
+      <c r="B56" s="20">
+        <v>21</v>
+      </c>
+      <c r="C56" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D56" s="20" t="s">
+        <v>1159</v>
+      </c>
+      <c r="E56" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F56" s="20">
+        <v>24</v>
+      </c>
+      <c r="G56" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H56" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I56" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J56" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K56" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A57" s="19">
+        <v>9</v>
+      </c>
+      <c r="B57" s="20">
+        <v>22</v>
+      </c>
+      <c r="C57" s="21" t="s">
+        <v>656</v>
+      </c>
+      <c r="D57" s="20" t="s">
+        <v>1153</v>
+      </c>
+      <c r="E57" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F57" s="20">
+        <v>24</v>
+      </c>
+      <c r="G57" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H57" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I57" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J57" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K57" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A58" s="19">
+        <v>9</v>
+      </c>
+      <c r="B58" s="20">
+        <v>23</v>
+      </c>
+      <c r="C58" s="21" t="s">
+        <v>1185</v>
+      </c>
+      <c r="D58" s="20" t="s">
+        <v>1202</v>
+      </c>
+      <c r="E58" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F58" s="20">
+        <v>24</v>
+      </c>
+      <c r="G58" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H58" s="21" t="s">
+        <v>3909</v>
+      </c>
+      <c r="I58" s="25" t="s">
+        <v>4293</v>
+      </c>
+      <c r="J58" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K58" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A59" s="19">
+        <v>9</v>
+      </c>
+      <c r="B59" s="20">
+        <v>24</v>
+      </c>
+      <c r="C59" s="21" t="s">
+        <v>4296</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>1191</v>
+      </c>
+      <c r="E59" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F59" s="10">
+        <v>24</v>
+      </c>
+      <c r="G59" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H59" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I59" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J59" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K59" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A60" s="19">
+        <v>9</v>
+      </c>
+      <c r="B60" s="20">
+        <v>25</v>
+      </c>
+      <c r="C60" s="21" t="s">
+        <v>1184</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>1203</v>
+      </c>
+      <c r="E60" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F60" s="20">
+        <v>24</v>
+      </c>
+      <c r="G60" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H60" s="21" t="s">
+        <v>3909</v>
+      </c>
+      <c r="I60" s="25" t="s">
+        <v>4293</v>
+      </c>
+      <c r="J60" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K60" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A61" s="19">
+        <v>9</v>
+      </c>
+      <c r="B61" s="20">
+        <v>26</v>
+      </c>
+      <c r="C61" s="21" t="s">
+        <v>1180</v>
+      </c>
+      <c r="D61" s="20" t="s">
+        <v>1206</v>
+      </c>
+      <c r="E61" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F61" s="10">
+        <v>24</v>
+      </c>
+      <c r="G61" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H61" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I61" s="20" t="s">
+        <v>4289</v>
+      </c>
+      <c r="J61" s="20" t="s">
+        <v>4290</v>
+      </c>
+      <c r="K61" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A62" s="19">
+        <v>9</v>
+      </c>
+      <c r="B62" s="20">
+        <v>27</v>
+      </c>
+      <c r="C62" s="21" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D62" s="20" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E62" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F62" s="10">
+        <v>12</v>
+      </c>
+      <c r="G62" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H62" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="I62" s="20" t="s">
+        <v>4292</v>
+      </c>
+      <c r="K62" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A63" s="19">
+        <v>9</v>
+      </c>
+      <c r="B63" s="20">
+        <v>27.1</v>
+      </c>
+      <c r="C63" s="21" t="s">
+        <v>3105</v>
+      </c>
+      <c r="D63" s="20" t="s">
+        <v>3106</v>
+      </c>
+      <c r="E63" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F63" s="20">
+        <v>12</v>
+      </c>
+      <c r="G63" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H63" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="I63" s="20" t="s">
+        <v>4292</v>
+      </c>
+      <c r="K63" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A64" s="19">
+        <v>9</v>
+      </c>
+      <c r="B64" s="20">
+        <v>27.2</v>
+      </c>
+      <c r="C64" s="21" t="s">
+        <v>3107</v>
+      </c>
+      <c r="D64" s="20" t="s">
+        <v>3108</v>
+      </c>
+      <c r="E64" s="26" t="s">
+        <v>4264</v>
+      </c>
+      <c r="F64" s="20">
+        <v>12</v>
+      </c>
+      <c r="G64" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H64" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="I64" s="20" t="s">
+        <v>4292</v>
+      </c>
+      <c r="K64" s="25">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D624538-775A-4896-8368-5AB97255472E}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:K63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -73094,7 +75623,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="18" t="s">
-        <v>4306</v>
+        <v>4304</v>
       </c>
       <c r="B1" s="22" t="s">
         <v>71</v>
@@ -73106,25 +75635,25 @@
         <v>1188</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>4307</v>
+        <v>4305</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>4315</v>
+        <v>4313</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>4308</v>
+        <v>4306</v>
       </c>
       <c r="H1" s="23" t="s">
         <v>78</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>4310</v>
+        <v>4308</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>4311</v>
+        <v>4309</v>
       </c>
       <c r="K1" s="24" t="s">
-        <v>4309</v>
+        <v>4307</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
@@ -74270,12 +76799,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="B31" sqref="B31:K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -74295,7 +76824,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="18" t="s">
-        <v>4306</v>
+        <v>4304</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>71</v>
@@ -74307,25 +76836,25 @@
         <v>1188</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>4307</v>
+        <v>4305</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>4315</v>
+        <v>4313</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>4308</v>
+        <v>4306</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>78</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>4310</v>
+        <v>4308</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>4311</v>
+        <v>4309</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>4309</v>
+        <v>4307</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
@@ -75354,7 +77883,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J9"/>
   <sheetViews>
@@ -75663,7 +78192,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
@@ -76110,294 +78639,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F3F6B6C-5426-41AC-9E1E-CFE1B1525272}">
-  <dimension ref="A1:D35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="65.73046875" customWidth="1"/>
-    <col min="2" max="2" width="11.86328125" customWidth="1"/>
-    <col min="3" max="3" width="12.59765625" customWidth="1"/>
-    <col min="4" max="4" width="13.86328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="27" t="s">
-        <v>4275</v>
-      </c>
-      <c r="C1" s="19"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="19" t="s">
-        <v>4276</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="27" t="s">
-        <v>4272</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>4273</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4301</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>4274</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4300</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>4277</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4305</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" s="19" t="s">
-        <v>4278</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>4302</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>4280</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4303</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" s="19" t="s">
-        <v>4287</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>4304</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A12" s="27" t="s">
-        <v>4279</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A13" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>4310</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>4311</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>4309</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A14" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>4289</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>4290</v>
-      </c>
-      <c r="D14" s="20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="21" t="s">
-        <v>3908</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>4290</v>
-      </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>4291</v>
-      </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A17" s="21" t="s">
-        <v>3905</v>
-      </c>
-      <c r="B17" s="25">
-        <v>1</v>
-      </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A18" s="21" t="s">
-        <v>3906</v>
-      </c>
-      <c r="B18" s="25">
-        <v>1</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>4290</v>
-      </c>
-      <c r="D18" s="20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>4292</v>
-      </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" s="21" t="s">
-        <v>3909</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>4293</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>4290</v>
-      </c>
-      <c r="D20" s="20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" s="21" t="s">
-        <v>3910</v>
-      </c>
-      <c r="B21" s="25">
-        <v>5</v>
-      </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22" s="21" t="s">
-        <v>3911</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>4293</v>
-      </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A23" s="21" t="s">
-        <v>3912</v>
-      </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="20" t="s">
-        <v>4291</v>
-      </c>
-      <c r="D23" s="20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="21" t="s">
-        <v>4288</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>4294</v>
-      </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A26" s="21" t="s">
-        <v>4312</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A27" s="21" t="s">
-        <v>4313</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A28" s="21" t="s">
-        <v>4314</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A30" s="27" t="s">
-        <v>4281</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A31" s="21" t="s">
-        <v>4282</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A32" s="21" t="s">
-        <v>4283</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A33" s="21" t="s">
-        <v>4286</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A34" s="21" t="s">
-        <v>4284</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A35" s="21" t="s">
-        <v>4285</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -76408,12 +78649,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010098C197DC67C0514EB308983AEF32E983" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a506a90b446ec8f6ca9341c1992a61de">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d55fa3f-3c18-425b-9faa-377f011f8097" xmlns:ns3="39d3cee1-f650-41e8-9a2f-4357c6682977" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="68eb73591874d7b6cee55945c0a8d5bf" ns2:_="" ns3:_="">
     <xsd:import namespace="3d55fa3f-3c18-425b-9faa-377f011f8097"/>
@@ -76590,6 +78825,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76AD4B54-6DC2-4D8C-86CA-5908AE6EF015}">
   <ds:schemaRefs>
@@ -76599,23 +78840,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC2EEFE0-2F39-4B6B-9A9A-7092F0DE0B00}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="3d55fa3f-3c18-425b-9faa-377f011f8097"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="39d3cee1-f650-41e8-9a2f-4357c6682977"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A61351A-2F7F-48FB-A782-AE9A92A10B40}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -76632,4 +78856,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC2EEFE0-2F39-4B6B-9A9A-7092F0DE0B00}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="3d55fa3f-3c18-425b-9faa-377f011f8097"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="39d3cee1-f650-41e8-9a2f-4357c6682977"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>